<commit_message>
added functions for xls unpacking and create EPG and create BD
</commit_message>
<xml_diff>
--- a/Create_EPG/EPG_Input.xlsx
+++ b/Create_EPG/EPG_Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Create_EPG</t>
   </si>
@@ -60,6 +60,39 @@
   </si>
   <si>
     <t>e7_L3_Out</t>
+  </si>
+  <si>
+    <t>Network_Mgmt</t>
+  </si>
+  <si>
+    <t>Tenant</t>
+  </si>
+  <si>
+    <t>ANP</t>
+  </si>
+  <si>
+    <t>Prod</t>
+  </si>
+  <si>
+    <t>e7_mgmt</t>
+  </si>
+  <si>
+    <t>VRF</t>
+  </si>
+  <si>
+    <t>Subnet</t>
+  </si>
+  <si>
+    <t>L3 out</t>
+  </si>
+  <si>
+    <t>advertise (yes/no)</t>
+  </si>
+  <si>
+    <t>10.207.50.1/24</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -374,57 +407,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.5" customWidth="1"/>
-    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="1" max="3" width="21.6640625" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
using xls variables for EPG and BD.
</commit_message>
<xml_diff>
--- a/Create_EPG/EPG_Input.xlsx
+++ b/Create_EPG/EPG_Input.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Create_EPG</t>
   </si>
@@ -50,15 +50,9 @@
     <t>Contract</t>
   </si>
   <si>
-    <t>Storage_Mgmt</t>
-  </si>
-  <si>
     <t>e7vmw1vic02</t>
   </si>
   <si>
-    <t>Storage_Mgmt_BD</t>
-  </si>
-  <si>
     <t>e7_L3_Out</t>
   </si>
   <si>
@@ -89,10 +83,25 @@
     <t>advertise (yes/no)</t>
   </si>
   <si>
-    <t>10.207.50.1/24</t>
-  </si>
-  <si>
-    <t>yes</t>
+    <t>PythonTest</t>
+  </si>
+  <si>
+    <t>PythonTest_BD</t>
+  </si>
+  <si>
+    <t>Py_Prod</t>
+  </si>
+  <si>
+    <t>10.207.250.1/24</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Py_test1</t>
+  </si>
+  <si>
+    <t>Py_mgmt</t>
   </si>
 </sst>
 </file>
@@ -410,7 +419,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -424,10 +433,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -450,65 +459,59 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
         <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
         <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
         <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -516,19 +519,19 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added function to create contract and filter
</commit_message>
<xml_diff>
--- a/Create_EPG/EPG_Input.xlsx
+++ b/Create_EPG/EPG_Input.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500"/>
+    <workbookView xWindow="7420" yWindow="1900" windowWidth="28800" windowHeight="16100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>Create_EPG</t>
   </si>
@@ -102,6 +102,42 @@
   </si>
   <si>
     <t>Py_mgmt</t>
+  </si>
+  <si>
+    <t>Create_Contract</t>
+  </si>
+  <si>
+    <t>Contract Name</t>
+  </si>
+  <si>
+    <t>Subject Name</t>
+  </si>
+  <si>
+    <t>Filter Name</t>
+  </si>
+  <si>
+    <t>Protocol</t>
+  </si>
+  <si>
+    <t>port</t>
+  </si>
+  <si>
+    <t>PythonWeb</t>
+  </si>
+  <si>
+    <t>PythonWebSubj</t>
+  </si>
+  <si>
+    <t>PythonWebFilter</t>
+  </si>
+  <si>
+    <t>tcp</t>
+  </si>
+  <si>
+    <t>https</t>
+  </si>
+  <si>
+    <t>Scope (VRF or Global)</t>
   </si>
 </sst>
 </file>
@@ -117,12 +153,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -137,8 +179,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -431,26 +474,26 @@
     <col min="7" max="7" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -494,23 +537,23 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -532,6 +575,55 @@
       </c>
       <c r="F6" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added print strings. Added contracts provided and consumed in EPG
</commit_message>
<xml_diff>
--- a/Create_EPG/EPG_Input.xlsx
+++ b/Create_EPG/EPG_Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7420" yWindow="1900" windowWidth="28800" windowHeight="16100" tabRatio="500"/>
+    <workbookView xWindow="2400" yWindow="1820" windowWidth="28800" windowHeight="16100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t>Create_EPG</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>Scope (VRF or Global)</t>
+  </si>
+  <si>
+    <t>Provide or Consume</t>
+  </si>
+  <si>
+    <t>consume</t>
   </si>
 </sst>
 </file>
@@ -459,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -474,7 +480,7 @@
     <col min="7" max="7" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
@@ -496,8 +502,11 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -513,11 +522,11 @@
       <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" t="s">
-        <v>8</v>
+      <c r="I2" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -537,7 +546,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
@@ -557,7 +566,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -577,7 +586,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
@@ -600,7 +609,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Added static path and Physical Domain
</commit_message>
<xml_diff>
--- a/Create_EPG/EPG_Input.xlsx
+++ b/Create_EPG/EPG_Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="1820" windowWidth="28800" windowHeight="16100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="28800" windowHeight="16100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>Create_EPG</t>
   </si>
@@ -144,6 +144,18 @@
   </si>
   <si>
     <t>consume</t>
+  </si>
+  <si>
+    <t>Physical_Domain</t>
+  </si>
+  <si>
+    <t>encap_vlan</t>
+  </si>
+  <si>
+    <t>E7_NETAPP</t>
+  </si>
+  <si>
+    <t>e7_NETAPP-A_VPC</t>
   </si>
 </sst>
 </file>
@@ -185,9 +197,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,22 +478,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="21.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.5" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
-    <col min="6" max="6" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="26.33203125" customWidth="1"/>
+    <col min="4" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="20.5" customWidth="1"/>
+    <col min="8" max="8" width="18.5" customWidth="1"/>
+    <col min="9" max="9" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
@@ -494,19 +507,25 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -519,14 +538,23 @@
       <c r="D2" t="s">
         <v>24</v>
       </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="2">
+        <v>800</v>
+      </c>
       <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -536,17 +564,17 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
@@ -556,17 +584,17 @@
       <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -579,14 +607,14 @@
       <c r="D6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>21</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
@@ -596,20 +624,20 @@
       <c r="D8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -622,16 +650,16 @@
       <c r="D9" t="s">
         <v>32</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>33</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>34</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>35</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>